<commit_message>
Added TryMe.txt. Modified Book1.xlsx
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitTest1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitTest2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Rita</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>Liza</t>
+  </si>
+  <si>
+    <t>Kukolka</t>
   </si>
 </sst>
 </file>
@@ -356,10 +359,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -389,6 +392,11 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>